<commit_message>
lecture 1 complete till VLOOKUP
</commit_message>
<xml_diff>
--- a/ExcelDataConsolidation/Input/Acquisitions.xlsx
+++ b/ExcelDataConsolidation/Input/Acquisitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolae.cocan\Documents\UiPath\Excel Data Consolidation\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\UiPath\ExcelDataConsolidation-rpa\ExcelDataConsolidation\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4907A8-D7FC-46E7-808B-B84D0DAD0C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0FB323-B8E3-4147-9433-0D8DB95B6A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40050" yWindow="465" windowWidth="8850" windowHeight="4590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisitions" sheetId="1" r:id="rId1"/>
@@ -1822,6 +1822,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
@@ -1830,15 +1839,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2084,20 +2084,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB9A8E1-E04D-4628-9179-505861E9CEB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
     <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB9A8E1-E04D-4628-9179-505861E9CEB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>